<commit_message>
i finished the filters in word list view, now i will been working in the view and edition of the word
</commit_message>
<xml_diff>
--- a/ionic-vocabulary/task/taskVocabulary.xlsx
+++ b/ionic-vocabulary/task/taskVocabulary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Function</t>
   </si>
@@ -55,13 +55,19 @@
   </si>
   <si>
     <t>Show filters actived</t>
+  </si>
+  <si>
+    <t>Show description of one word</t>
+  </si>
+  <si>
+    <t>DEVELOPING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +90,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +108,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,20 +135,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
     <cellStyle name="Buena" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
@@ -431,30 +463,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -462,7 +495,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -470,7 +503,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -481,7 +514,7 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -491,13 +524,24 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -519,15 +563,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i continue developing vocabulary module
</commit_message>
<xml_diff>
--- a/ionic-vocabulary/task/taskVocabulary.xlsx
+++ b/ionic-vocabulary/task/taskVocabulary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Function</t>
   </si>
@@ -51,9 +51,6 @@
     <t>When we define the word, we need to show the new word in the view</t>
   </si>
   <si>
-    <t>We to check the validation when we want to save one verb and this does not have its conjugation</t>
-  </si>
-  <si>
     <t>Show filters actived</t>
   </si>
   <si>
@@ -61,6 +58,45 @@
   </si>
   <si>
     <t>DEVELOPING</t>
+  </si>
+  <si>
+    <t>Save word per user</t>
+  </si>
+  <si>
+    <t>Each user has own words</t>
+  </si>
+  <si>
+    <t>Overwirte own word</t>
+  </si>
+  <si>
+    <t>When an user has overwritten own word, the system have to overwrite that word</t>
+  </si>
+  <si>
+    <t>when we syncronize your words you can segment this with an identifier</t>
+  </si>
+  <si>
+    <t>remove the word filter when is new new word view</t>
+  </si>
+  <si>
+    <t>when I create a new word or update a existing word, I need to refresh the dictionary</t>
+  </si>
+  <si>
+    <t>when we delete a verb definition when need to put all verb fields in blank</t>
+  </si>
+  <si>
+    <t>remove el publish word:updated after we used it</t>
+  </si>
+  <si>
+    <t>delete word</t>
+  </si>
+  <si>
+    <t>when I delete a existing word, I need to refresh the dictionary</t>
+  </si>
+  <si>
+    <t>The words are saving twice</t>
+  </si>
+  <si>
+    <t>when we add N words, we need to create an array and publishing</t>
   </si>
 </sst>
 </file>
@@ -98,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +150,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -135,13 +176,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,10 +201,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
     <cellStyle name="Buena" xfId="2" builtinId="26"/>
+    <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
@@ -463,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,10 +571,13 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -538,10 +585,69 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +660,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,9 +676,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -582,12 +688,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i fixed bug in vocabulary module
</commit_message>
<xml_diff>
--- a/ionic-vocabulary/task/taskVocabulary.xlsx
+++ b/ionic-vocabulary/task/taskVocabulary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Function</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>when we add N words, we need to create an array and publishing</t>
+  </si>
+  <si>
+    <t>when I create a market or discusion module I need to include a help section when the estudents can publis their doubst about one word or grammar</t>
+  </si>
+  <si>
+    <t>I need to add an internal id to each word</t>
+  </si>
+  <si>
+    <t>IMPORTANT</t>
   </si>
 </sst>
 </file>
@@ -507,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +636,6 @@
       <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -648,6 +656,19 @@
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i am working in the notifications words
</commit_message>
<xml_diff>
--- a/ionic-vocabulary/task/taskVocabulary.xlsx
+++ b/ionic-vocabulary/task/taskVocabulary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Function</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Show description of one word</t>
   </si>
   <si>
-    <t>DEVELOPING</t>
-  </si>
-  <si>
     <t>Save word per user</t>
   </si>
   <si>
@@ -103,16 +100,13 @@
   </si>
   <si>
     <t>I need to add an internal id to each word</t>
-  </si>
-  <si>
-    <t>IMPORTANT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,15 +129,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,17 +140,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -185,14 +161,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -207,15 +181,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
+  <cellStyles count="3">
     <cellStyle name="Buena" xfId="2" builtinId="26"/>
-    <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
@@ -519,7 +487,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,18 +564,18 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -615,7 +583,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -623,7 +591,7 @@
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
@@ -631,7 +599,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -639,7 +607,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>8</v>
@@ -647,7 +615,7 @@
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
@@ -655,20 +623,23 @@
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>29</v>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +670,7 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -738,18 +709,18 @@
     </row>
     <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i add new a super market list module, i need to do many improvements but i have a simple version of this module
</commit_message>
<xml_diff>
--- a/ionic-vocabulary/task/taskVocabulary.xlsx
+++ b/ionic-vocabulary/task/taskVocabulary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Function</t>
   </si>
@@ -100,13 +100,19 @@
   </si>
   <si>
     <t>I need to add an internal id to each word</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>DEVELOPING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +135,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +156,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,13 +179,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -181,9 +216,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Buena" xfId="2" builtinId="26"/>
+    <cellStyle name="Cálculo" xfId="3" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
@@ -484,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,6 +679,14 @@
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>